<commit_message>
Minor updates after 10/31 meeting
</commit_message>
<xml_diff>
--- a/GCMP_md_forGEOME_v2.xlsx
+++ b/GCMP_md_forGEOME_v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/github/GCMP2GEOME/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edc5240/github/GCMP2GEOME/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CF0348-E211-664B-B6BB-5F72595610B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126F590A-CAAD-0C4D-A6C0-FADDCA60CCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="500" windowWidth="31980" windowHeight="16240" xr2:uid="{97506BC2-AB4A-0C4B-AE34-BE9DA0630CE3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="259">
   <si>
     <t>GCMP</t>
   </si>
@@ -1190,6 +1190,12 @@
   </si>
   <si>
     <t>basisOfRecord</t>
+  </si>
+  <si>
+    <t>red, blue, green</t>
+  </si>
+  <si>
+    <t>0 - 500</t>
   </si>
 </sst>
 </file>
@@ -1358,7 +1364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1376,7 +1382,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1699,9 +1704,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A07CDAA-BE66-D94A-8019-C7B9FC938BA8}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="245" zoomScaleNormal="245" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C9" sqref="C9"/>
+      <selection pane="topRight" activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1746,7 +1751,7 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
@@ -1803,7 +1808,7 @@
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C5" t="s">
@@ -1823,7 +1828,7 @@
       <c r="A6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C6" t="s">
@@ -1843,7 +1848,7 @@
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>256</v>
       </c>
       <c r="C7" t="s">
@@ -1877,7 +1882,7 @@
       <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>42</v>
       </c>
       <c r="C9" t="s">
@@ -1902,7 +1907,7 @@
       <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>48</v>
       </c>
       <c r="C11" t="s">
@@ -1933,7 +1938,7 @@
       <c r="A13" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>56</v>
       </c>
       <c r="C13" t="s">
@@ -1947,7 +1952,7 @@
       <c r="A14" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C14" t="s">
@@ -1961,7 +1966,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>62</v>
       </c>
       <c r="C15" t="s">
@@ -1973,7 +1978,7 @@
       <c r="A16" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>64</v>
       </c>
       <c r="C16" t="s">
@@ -2007,7 +2012,7 @@
       <c r="A18" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>70</v>
       </c>
       <c r="C18" t="s">
@@ -2024,7 +2029,7 @@
       <c r="A19" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>73</v>
       </c>
       <c r="C19" t="s">
@@ -2038,7 +2043,7 @@
       <c r="A20" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>76</v>
       </c>
       <c r="C20" t="s">
@@ -2052,7 +2057,7 @@
       <c r="A21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="17" t="s">
         <v>79</v>
       </c>
       <c r="C21" t="s">
@@ -2069,7 +2074,7 @@
       <c r="A22" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>82</v>
       </c>
       <c r="C22" t="s">
@@ -2100,7 +2105,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>89</v>
       </c>
       <c r="C24" t="s">
@@ -2137,7 +2142,7 @@
       <c r="A26" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>97</v>
       </c>
       <c r="C26" t="s">
@@ -2157,7 +2162,7 @@
       <c r="A27" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="17" t="s">
         <v>102</v>
       </c>
       <c r="C27" t="s">
@@ -2177,7 +2182,7 @@
       <c r="A28" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="17" t="s">
         <v>106</v>
       </c>
       <c r="C28" t="s">
@@ -2191,7 +2196,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="13" t="s">
+      <c r="A29" t="s">
         <v>109</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -2205,7 +2210,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
+      <c r="A30" t="s">
         <v>111</v>
       </c>
       <c r="B30" s="12" t="s">
@@ -2222,7 +2227,7 @@
       <c r="A31" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="16" t="s">
         <v>115</v>
       </c>
       <c r="C31" t="s">
@@ -2239,7 +2244,7 @@
       <c r="A32" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>118</v>
       </c>
       <c r="C32" t="s">
@@ -2256,7 +2261,7 @@
       <c r="A33" t="s">
         <v>120</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>212</v>
       </c>
       <c r="C33" t="s">
@@ -2273,7 +2278,7 @@
       <c r="A34" t="s">
         <v>122</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>255</v>
       </c>
       <c r="C34" t="s">
@@ -2290,7 +2295,6 @@
       <c r="A35" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B35" s="13"/>
       <c r="H35" s="5" t="s">
         <v>125</v>
       </c>
@@ -2299,7 +2303,6 @@
       <c r="A36" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B36" s="13"/>
       <c r="H36" s="5" t="s">
         <v>125</v>
       </c>
@@ -2308,7 +2311,7 @@
       <c r="A37" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>214</v>
       </c>
       <c r="C37" t="s">
@@ -2325,7 +2328,7 @@
       <c r="A38" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="13" t="s">
         <v>215</v>
       </c>
       <c r="C38" t="s">
@@ -2342,7 +2345,7 @@
       <c r="A39" t="s">
         <v>130</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="13" t="s">
         <v>216</v>
       </c>
       <c r="C39" t="s">
@@ -2392,7 +2395,7 @@
       <c r="A43" t="s">
         <v>139</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="13" t="s">
         <v>218</v>
       </c>
       <c r="C43" t="s">
@@ -2400,6 +2403,9 @@
       </c>
       <c r="D43" t="s">
         <v>226</v>
+      </c>
+      <c r="E43" t="s">
+        <v>258</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>140</v>
@@ -2409,7 +2415,7 @@
       <c r="A44" t="s">
         <v>141</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="13" t="s">
         <v>219</v>
       </c>
       <c r="C44" t="s">
@@ -2426,7 +2432,7 @@
       <c r="A45" t="s">
         <v>143</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="13" t="s">
         <v>220</v>
       </c>
       <c r="C45" t="s">
@@ -2443,7 +2449,7 @@
       <c r="A46" t="s">
         <v>145</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="13" t="s">
         <v>221</v>
       </c>
       <c r="C46" t="s">
@@ -2451,6 +2457,9 @@
       </c>
       <c r="D46" t="s">
         <v>225</v>
+      </c>
+      <c r="E46" t="s">
+        <v>257</v>
       </c>
       <c r="G46" t="s">
         <v>146</v>
@@ -2463,7 +2472,7 @@
       <c r="A47" t="s">
         <v>148</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="13" t="s">
         <v>222</v>
       </c>
       <c r="C47" t="s">
@@ -2480,7 +2489,7 @@
       <c r="A48" t="s">
         <v>150</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
         <v>223</v>
       </c>
       <c r="C48" t="s">
@@ -2497,7 +2506,7 @@
       <c r="A49" t="s">
         <v>152</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="13" t="s">
         <v>227</v>
       </c>
       <c r="C49" t="s">
@@ -2514,7 +2523,7 @@
       <c r="A50" t="s">
         <v>154</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>228</v>
       </c>
       <c r="C50" t="s">
@@ -2531,7 +2540,7 @@
       <c r="A51" t="s">
         <v>156</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="13" t="s">
         <v>232</v>
       </c>
       <c r="C51" t="s">
@@ -2548,7 +2557,7 @@
       <c r="A52" t="s">
         <v>158</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="13" t="s">
         <v>229</v>
       </c>
       <c r="C52" t="s">
@@ -2565,7 +2574,7 @@
       <c r="A53" t="s">
         <v>160</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="13" t="s">
         <v>231</v>
       </c>
       <c r="C53" t="s">
@@ -2582,7 +2591,7 @@
       <c r="A54" t="s">
         <v>162</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="13" t="s">
         <v>230</v>
       </c>
       <c r="C54" t="s">
@@ -2599,7 +2608,7 @@
       <c r="A55" t="s">
         <v>164</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="13" t="s">
         <v>233</v>
       </c>
       <c r="C55" t="s">
@@ -2616,7 +2625,7 @@
       <c r="A56" t="s">
         <v>166</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="13" t="s">
         <v>234</v>
       </c>
       <c r="C56" t="s">
@@ -2633,7 +2642,7 @@
       <c r="A57" t="s">
         <v>168</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="13" t="s">
         <v>235</v>
       </c>
       <c r="C57" t="s">
@@ -2650,7 +2659,7 @@
       <c r="A58" t="s">
         <v>170</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="13" t="s">
         <v>238</v>
       </c>
       <c r="C58" t="s">
@@ -2667,7 +2676,7 @@
       <c r="A59" t="s">
         <v>172</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="13" t="s">
         <v>236</v>
       </c>
       <c r="C59" t="s">
@@ -2684,7 +2693,7 @@
       <c r="A60" t="s">
         <v>174</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="13" t="s">
         <v>237</v>
       </c>
       <c r="C60" t="s">
@@ -2701,7 +2710,7 @@
       <c r="A61" t="s">
         <v>176</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="13" t="s">
         <v>239</v>
       </c>
       <c r="C61" t="s">
@@ -2718,7 +2727,7 @@
       <c r="A62" t="s">
         <v>178</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="13" t="s">
         <v>240</v>
       </c>
       <c r="C62" t="s">
@@ -2732,7 +2741,7 @@
       <c r="A63" t="s">
         <v>180</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="13" t="s">
         <v>241</v>
       </c>
       <c r="C63" t="s">
@@ -2749,7 +2758,7 @@
       <c r="A64" t="s">
         <v>182</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="13" t="s">
         <v>242</v>
       </c>
       <c r="C64" t="s">
@@ -2766,7 +2775,7 @@
       <c r="A65" t="s">
         <v>184</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="13" t="s">
         <v>243</v>
       </c>
       <c r="C65" t="s">
@@ -2783,7 +2792,7 @@
       <c r="A66" t="s">
         <v>186</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="13" t="s">
         <v>244</v>
       </c>
       <c r="C66" t="s">
@@ -2800,7 +2809,7 @@
       <c r="A67" t="s">
         <v>188</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="13" t="s">
         <v>245</v>
       </c>
       <c r="C67" t="s">
@@ -2814,7 +2823,7 @@
       <c r="A68" t="s">
         <v>190</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="13" t="s">
         <v>246</v>
       </c>
       <c r="C68" t="s">
@@ -2828,7 +2837,7 @@
       <c r="A69" t="s">
         <v>192</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="13" t="s">
         <v>247</v>
       </c>
       <c r="C69" t="s">
@@ -2845,7 +2854,7 @@
       <c r="A70" t="s">
         <v>194</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="13" t="s">
         <v>248</v>
       </c>
       <c r="C70" t="s">
@@ -2859,7 +2868,7 @@
       <c r="A71" t="s">
         <v>196</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="13" t="s">
         <v>249</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -2872,7 +2881,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B72" s="15" t="s">
+      <c r="B72" s="14" t="s">
         <v>198</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -2888,7 +2897,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="15" t="s">
         <v>200</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -3007,12 +3016,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064906E29D34BD94BBAB6F6B683A96120" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="83c122223da3a1705a199869f9ecf5e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3effcad5-9b97-44a0-b712-3d5e8f84c098" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79e503b41c506afe4cbe028f024791ea" ns2:_="">
     <xsd:import namespace="3effcad5-9b97-44a0-b712-3d5e8f84c098"/>
@@ -3196,6 +3199,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0ED0312-E49C-4DB7-A97A-581D026BC90B}">
   <ds:schemaRefs>
@@ -3205,15 +3214,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DC8E859-26CB-4CED-A136-6D5D5B2B3A6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFDE0778-F960-4F65-8A23-D1F13E31406E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3229,4 +3229,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DC8E859-26CB-4CED-A136-6D5D5B2B3A6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Deprecate some files and update a to-do list to address first round of errors in validation
</commit_message>
<xml_diff>
--- a/GCMP_md_forGEOME_v2.xlsx
+++ b/GCMP_md_forGEOME_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edc5240/github/GCMP2GEOME/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126F590A-CAAD-0C4D-A6C0-FADDCA60CCEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C38331-76D7-274C-88D7-7964BA2E5131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="500" windowWidth="31980" windowHeight="16240" xr2:uid="{97506BC2-AB4A-0C4B-AE34-BE9DA0630CE3}"/>
+    <workbookView xWindow="45220" yWindow="7060" windowWidth="31980" windowHeight="16240" xr2:uid="{97506BC2-AB4A-0C4B-AE34-BE9DA0630CE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={3D945AA6-E6A7-5045-B56A-B6ACF48D7F3C}</author>
+  </authors>
+  <commentList>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{3D945AA6-E6A7-5045-B56A-B6ACF48D7F3C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Find a new field for sample type, and use appropriate vocab for basisOfRecord</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="259">
   <si>
@@ -1202,7 +1220,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1296,6 +1314,12 @@
       <name val="Verdana"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1405,10 +1429,16 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Crandall, Eric" id="{5CB24955-793E-0B40-BB07-7E8B03352B0F}" userId="S::edc5240@psu.edu::b71e483b-5258-4141-a063-b7adf4ca072d" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1446,7 +1476,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1552,7 +1582,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1694,19 +1724,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B7" dT="2024-05-15T14:15:10.31" personId="{5CB24955-793E-0B40-BB07-7E8B03352B0F}" id="{3D945AA6-E6A7-5045-B56A-B6ACF48D7F3C}">
+    <text>Find a new field for sample type, and use appropriate vocab for basisOfRecord</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A07CDAA-BE66-D94A-8019-C7B9FC938BA8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A07CDAA-BE66-D94A-8019-C7B9FC938BA8}">
   <dimension ref="A1:H77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="245" zoomScaleNormal="245" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="245" zoomScaleNormal="245" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A55" sqref="A55"/>
+      <selection pane="topRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2932,6 +2970,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -3007,12 +3046,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3200,15 +3236,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0ED0312-E49C-4DB7-A97A-581D026BC90B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DC8E859-26CB-4CED-A136-6D5D5B2B3A6A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3232,10 +3272,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DC8E859-26CB-4CED-A136-6D5D5B2B3A6A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0ED0312-E49C-4DB7-A97A-581D026BC90B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update data loading and renaming code to get the outputs to load into GEOME
</commit_message>
<xml_diff>
--- a/GCMP_md_forGEOME_v2.xlsx
+++ b/GCMP_md_forGEOME_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edc5240/github/GCMP2GEOME/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric/github/GCMP2GEOME/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C38331-76D7-274C-88D7-7964BA2E5131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D82164A-6FFC-4447-ADD2-D9D69CB4B65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45220" yWindow="7060" windowWidth="31980" windowHeight="16240" xr2:uid="{97506BC2-AB4A-0C4B-AE34-BE9DA0630CE3}"/>
+    <workbookView xWindow="51200" yWindow="7060" windowWidth="31980" windowHeight="16240" xr2:uid="{97506BC2-AB4A-0C4B-AE34-BE9DA0630CE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,65 @@
   <commentList>
     <comment ref="B7" authorId="0" shapeId="0" xr:uid="{3D945AA6-E6A7-5045-B56A-B6ACF48D7F3C}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Find a new field for sample type, and use appropriate vocab for basisOfRecord</t>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Comment:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    Find a new field for sample type, and use appropriate vocab for basisOfRecord</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -1220,7 +1275,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1315,12 +1370,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -1388,7 +1437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1407,7 +1456,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -1436,9 +1484,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1476,7 +1524,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1582,7 +1630,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1724,7 +1772,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1744,7 +1792,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="245" zoomScaleNormal="245" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B7" sqref="B7"/>
+      <selection pane="topRight" activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1789,7 +1837,7 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C2" t="s">
@@ -1846,7 +1894,7 @@
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>24</v>
       </c>
       <c r="C5" t="s">
@@ -1866,7 +1914,7 @@
       <c r="A6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>29</v>
       </c>
       <c r="C6" t="s">
@@ -1886,7 +1934,7 @@
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>256</v>
       </c>
       <c r="C7" t="s">
@@ -1920,7 +1968,7 @@
       <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C9" t="s">
@@ -1945,7 +1993,7 @@
       <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C11" t="s">
@@ -1976,7 +2024,7 @@
       <c r="A13" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>56</v>
       </c>
       <c r="C13" t="s">
@@ -1990,7 +2038,7 @@
       <c r="A14" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>59</v>
       </c>
       <c r="C14" t="s">
@@ -2004,7 +2052,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>62</v>
       </c>
       <c r="C15" t="s">
@@ -2016,7 +2064,7 @@
       <c r="A16" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C16" t="s">
@@ -2050,7 +2098,7 @@
       <c r="A18" t="s">
         <v>70</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="16" t="s">
         <v>70</v>
       </c>
       <c r="C18" t="s">
@@ -2067,7 +2115,7 @@
       <c r="A19" t="s">
         <v>72</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>73</v>
       </c>
       <c r="C19" t="s">
@@ -2081,7 +2129,7 @@
       <c r="A20" t="s">
         <v>75</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="16" t="s">
         <v>76</v>
       </c>
       <c r="C20" t="s">
@@ -2095,7 +2143,7 @@
       <c r="A21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C21" t="s">
@@ -2112,7 +2160,7 @@
       <c r="A22" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="16" t="s">
         <v>82</v>
       </c>
       <c r="C22" t="s">
@@ -2143,7 +2191,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="15" t="s">
         <v>89</v>
       </c>
       <c r="C24" t="s">
@@ -2180,7 +2228,7 @@
       <c r="A26" t="s">
         <v>96</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="15" t="s">
         <v>97</v>
       </c>
       <c r="C26" t="s">
@@ -2200,7 +2248,7 @@
       <c r="A27" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>102</v>
       </c>
       <c r="C27" t="s">
@@ -2220,7 +2268,7 @@
       <c r="A28" t="s">
         <v>105</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>106</v>
       </c>
       <c r="C28" t="s">
@@ -2265,7 +2313,7 @@
       <c r="A31" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>115</v>
       </c>
       <c r="C31" t="s">
@@ -2282,7 +2330,7 @@
       <c r="A32" t="s">
         <v>117</v>
       </c>
-      <c r="B32" s="16" t="s">
+      <c r="B32" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C32" t="s">
@@ -2906,7 +2954,7 @@
       <c r="A71" t="s">
         <v>196</v>
       </c>
-      <c r="B71" s="13" t="s">
+      <c r="B71" s="15" t="s">
         <v>249</v>
       </c>
       <c r="C71" s="1" t="s">
@@ -2919,7 +2967,7 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="15" t="s">
         <v>198</v>
       </c>
       <c r="C72" s="1" t="s">
@@ -2935,7 +2983,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="15" t="s">
+      <c r="B73" s="14" t="s">
         <v>200</v>
       </c>
       <c r="C73" s="1" t="s">
@@ -3052,6 +3100,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064906E29D34BD94BBAB6F6B683A96120" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="83c122223da3a1705a199869f9ecf5e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3effcad5-9b97-44a0-b712-3d5e8f84c098" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="79e503b41c506afe4cbe028f024791ea" ns2:_="">
     <xsd:import namespace="3effcad5-9b97-44a0-b712-3d5e8f84c098"/>
@@ -3235,15 +3292,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DC8E859-26CB-4CED-A136-6D5D5B2B3A6A}">
   <ds:schemaRefs>
@@ -3254,6 +3302,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0ED0312-E49C-4DB7-A97A-581D026BC90B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FFDE0778-F960-4F65-8A23-D1F13E31406E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3269,12 +3325,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0ED0312-E49C-4DB7-A97A-581D026BC90B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>